<commit_message>
Uppdated XPS data files
</commit_message>
<xml_diff>
--- a/Data/XPS/control.xlsx
+++ b/Data/XPS/control.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22188" windowHeight="9180" activeTab="2"/>
+    <workbookView windowWidth="25600" windowHeight="12080"/>
   </bookViews>
   <sheets>
     <sheet name="I3d Scan A" sheetId="15" r:id="rId1"/>
@@ -12,22 +12,28 @@
     <sheet name="Pb4f Scan A" sheetId="13" r:id="rId3"/>
     <sheet name="O1s Scan A" sheetId="12" r:id="rId4"/>
     <sheet name="N1s Scan A" sheetId="11" r:id="rId5"/>
-    <sheet name="Titles A" sheetId="10" r:id="rId6"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId7"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId8"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="33">
   <si>
     <t>Acquisition Parameters :</t>
-  </si>
-  <si>
-    <t xml:space="preserve">聀 </t>
   </si>
   <si>
     <t xml:space="preserve">  </t>
@@ -39,9 +45,6 @@
     <t>6 mins 0.5 secs</t>
   </si>
   <si>
-    <t xml:space="preserve">k?p </t>
-  </si>
-  <si>
     <t>﻿</t>
   </si>
   <si>
@@ -51,37 +54,16 @@
     <t>Al K Alpha</t>
   </si>
   <si>
-    <t xml:space="preserve">轴 </t>
-  </si>
-  <si>
     <t>Energy</t>
   </si>
   <si>
     <t>Elements=</t>
   </si>
   <si>
-    <t>I?_x000f_</t>
-  </si>
-  <si>
-    <t>500 祄</t>
-  </si>
-  <si>
-    <t>_x000f_\!_x000f_</t>
-  </si>
-  <si>
     <t>Standard</t>
   </si>
   <si>
-    <t>E:\chenchen-4\chenchen-1\control.DATA\I3d Scan_2.VGD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_x0006_愱!_x000f_ </t>
-  </si>
-  <si>
     <t>CAE : Pass Energy 20.0 eV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">e </t>
   </si>
   <si>
     <t>0.050 eV</t>
@@ -117,9 +99,6 @@
     <t>3 mins 48.5 secs</t>
   </si>
   <si>
-    <t>E:\chenchen-4\chenchen-1\control.DATA\C1s Scan_2.VGD</t>
-  </si>
-  <si>
     <t>C1s</t>
   </si>
   <si>
@@ -132,9 +111,6 @@
     <t>2 mins 0.3 secs</t>
   </si>
   <si>
-    <t>E:\chenchen-4\chenchen-1\control.DATA\Pb4f Scan_2.VGD</t>
-  </si>
-  <si>
     <t>Pb4f</t>
   </si>
   <si>
@@ -142,9 +118,6 @@
   </si>
   <si>
     <t>1 mins 30.3 secs</t>
-  </si>
-  <si>
-    <t>E:\chenchen-4\chenchen-1\control.DATA\O1s Scan_2.VGD</t>
   </si>
   <si>
     <t>O1s</t>
@@ -156,52 +129,13 @@
     <t>5 mins 24.8 secs</t>
   </si>
   <si>
-    <t>E:\chenchen-4\chenchen-1\control.DATA\N1s Scan_2.VGD</t>
-  </si>
-  <si>
     <t>N1s</t>
-  </si>
-  <si>
-    <t>14:41:56  Tuesday, December 12, 2023</t>
-  </si>
-  <si>
-    <t>E:\chenchen-4\chenchen-1\control.xlsx</t>
-  </si>
-  <si>
-    <t>control</t>
-  </si>
-  <si>
-    <t>数据文件  :</t>
-  </si>
-  <si>
-    <t>标题</t>
-  </si>
-  <si>
-    <t>文件名</t>
-  </si>
-  <si>
-    <t>评论</t>
-  </si>
-  <si>
-    <t>I3d Scan</t>
-  </si>
-  <si>
-    <t>C1s Scan</t>
-  </si>
-  <si>
-    <t>Pb4f Scan</t>
-  </si>
-  <si>
-    <t>O1s Scan</t>
-  </si>
-  <si>
-    <t>N1s Scan</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
   <numFmts count="4">
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
@@ -927,8 +861,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14773275" y="3886200"/>
-          <a:ext cx="3065145" cy="3512820"/>
+          <a:off x="15022830" y="3779520"/>
+          <a:ext cx="3145155" cy="3416300"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -987,8 +921,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13458825" y="2926080"/>
-          <a:ext cx="3065145" cy="3512820"/>
+          <a:off x="13708380" y="2844800"/>
+          <a:ext cx="3105150" cy="3416300"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1047,8 +981,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13536295" y="2926080"/>
-          <a:ext cx="3065145" cy="3512820"/>
+          <a:off x="13787120" y="2844800"/>
+          <a:ext cx="3105150" cy="3416300"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1107,8 +1041,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14076045" y="2926080"/>
-          <a:ext cx="3048000" cy="3512820"/>
+          <a:off x="14338300" y="2844800"/>
+          <a:ext cx="3091180" cy="3416300"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1167,8 +1101,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13458825" y="2926080"/>
-          <a:ext cx="3065145" cy="3512820"/>
+          <a:off x="13708380" y="2844800"/>
+          <a:ext cx="3105150" cy="3416300"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1442,13 +1376,13 @@
   <sheetPr/>
   <dimension ref="A1:I617"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15:F15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4:H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="58.25" customWidth="1"/>
+    <col min="1" max="1" width="58.2545454545455" customWidth="1"/>
     <col min="2" max="2" width="7.5" customWidth="1"/>
     <col min="3" max="3" width="31.5" customWidth="1"/>
     <col min="4" max="4" width="4.5" customWidth="1"/>
@@ -1460,91 +1394,67 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="8:9">
-      <c r="H3" t="s">
+    <row r="3" spans="9:9">
+      <c r="I3" t="s">
         <v>1</v>
-      </c>
-      <c r="I3" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="4" spans="8:9">
       <c r="H4" t="s">
+        <v>2</v>
+      </c>
+      <c r="I4" t="s">
         <v>3</v>
       </c>
-      <c r="I4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="8:9">
-      <c r="H5" t="s">
-        <v>5</v>
-      </c>
+    </row>
+    <row r="5" spans="9:9">
       <c r="I5">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H6" t="s">
+        <v>5</v>
+      </c>
+      <c r="I6" t="s">
         <v>6</v>
       </c>
-      <c r="H6" t="s">
+    </row>
+    <row r="7" spans="2:9">
+      <c r="B7" t="s">
         <v>7</v>
       </c>
-      <c r="I6" t="s">
+      <c r="C7" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" t="s">
-        <v>11</v>
       </c>
       <c r="D7">
         <v>601</v>
       </c>
-      <c r="H7" t="s">
-        <v>12</v>
-      </c>
-      <c r="I7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="8:9">
-      <c r="H8" t="s">
-        <v>14</v>
-      </c>
+      <c r="I7">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="8" spans="9:9">
       <c r="I8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H9" t="s">
-        <v>17</v>
-      </c>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="9:9">
       <c r="I9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="8:9">
-      <c r="H10" t="s">
-        <v>19</v>
-      </c>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="9:9">
       <c r="I10" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="8:9">
       <c r="H11" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="I11">
         <v>601</v>
@@ -1552,45 +1462,45 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="E15" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="F15" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="G15" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="H15" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="I15" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="C16" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="E16" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="F16" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="G16" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="H16" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="I16" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -15428,13 +15338,13 @@
   <sheetPr/>
   <dimension ref="A1:I397"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4:H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="58.25" customWidth="1"/>
+    <col min="1" max="1" width="58.2545454545455" customWidth="1"/>
     <col min="2" max="2" width="7.5" customWidth="1"/>
     <col min="3" max="3" width="31.5" customWidth="1"/>
     <col min="4" max="4" width="4.5" customWidth="1"/>
@@ -15446,91 +15356,67 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="8:9">
-      <c r="H3" t="s">
+    <row r="3" spans="9:9">
+      <c r="I3" t="s">
         <v>1</v>
-      </c>
-      <c r="I3" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="4" spans="8:9">
       <c r="H4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="8:9">
-      <c r="H5" t="s">
-        <v>5</v>
-      </c>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="9:9">
       <c r="I5">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H6" t="s">
+        <v>5</v>
+      </c>
+      <c r="I6" t="s">
         <v>6</v>
       </c>
-      <c r="H6" t="s">
+    </row>
+    <row r="7" spans="2:9">
+      <c r="B7" t="s">
         <v>7</v>
       </c>
-      <c r="I6" t="s">
+      <c r="C7" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" t="s">
-        <v>11</v>
       </c>
       <c r="D7">
         <v>381</v>
       </c>
-      <c r="H7" t="s">
-        <v>12</v>
-      </c>
-      <c r="I7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="8:9">
-      <c r="H8" t="s">
-        <v>14</v>
-      </c>
+      <c r="I7">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="8" spans="9:9">
       <c r="I8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" t="s">
-        <v>31</v>
-      </c>
-      <c r="H9" t="s">
-        <v>17</v>
-      </c>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="9:9">
       <c r="I9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="8:9">
-      <c r="H10" t="s">
-        <v>19</v>
-      </c>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="9:9">
       <c r="I10" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="8:9">
       <c r="H11" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="I11">
         <v>381</v>
@@ -15538,45 +15424,45 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" t="s">
         <v>22</v>
       </c>
-      <c r="E15" t="s">
-        <v>32</v>
-      </c>
       <c r="F15" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="G15" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="H15" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="I15" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="C16" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="E16" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="F16" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="G16" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="H16" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="I16" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -24354,13 +24240,13 @@
   <sheetPr/>
   <dimension ref="A1:I417"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A389" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:H417"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="59.3796296296296" customWidth="1"/>
+    <col min="1" max="1" width="59.3818181818182" customWidth="1"/>
     <col min="2" max="2" width="7.5" customWidth="1"/>
     <col min="3" max="3" width="31.5" customWidth="1"/>
     <col min="4" max="4" width="4.5" customWidth="1"/>
@@ -24372,91 +24258,67 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="8:9">
-      <c r="H3" t="s">
+    <row r="3" spans="9:9">
+      <c r="I3" t="s">
         <v>1</v>
-      </c>
-      <c r="I3" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="4" spans="8:9">
       <c r="H4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="8:9">
-      <c r="H5" t="s">
-        <v>5</v>
-      </c>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="9:9">
       <c r="I5">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H6" t="s">
+        <v>5</v>
+      </c>
+      <c r="I6" t="s">
         <v>6</v>
       </c>
-      <c r="H6" t="s">
+    </row>
+    <row r="7" spans="2:9">
+      <c r="B7" t="s">
         <v>7</v>
       </c>
-      <c r="I6" t="s">
+      <c r="C7" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" t="s">
-        <v>11</v>
       </c>
       <c r="D7">
         <v>401</v>
       </c>
-      <c r="H7" t="s">
-        <v>12</v>
-      </c>
-      <c r="I7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="8:9">
-      <c r="H8" t="s">
-        <v>14</v>
-      </c>
+      <c r="I7">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="8" spans="9:9">
       <c r="I8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" t="s">
-        <v>36</v>
-      </c>
-      <c r="H9" t="s">
-        <v>17</v>
-      </c>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="9:9">
       <c r="I9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="8:9">
-      <c r="H10" t="s">
-        <v>19</v>
-      </c>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="9:9">
       <c r="I10" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="8:9">
       <c r="H11" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="I11">
         <v>401</v>
@@ -24464,45 +24326,45 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="E15" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="F15" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="G15" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="H15" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="I15" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="C16" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="E16" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="F16" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="G16" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="H16" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="I16" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -33740,18 +33602,18 @@
   <sheetPr/>
   <dimension ref="A1:I317"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="58.25" customWidth="1"/>
+    <col min="1" max="1" width="58.2545454545455" customWidth="1"/>
     <col min="2" max="2" width="7.5" customWidth="1"/>
-    <col min="3" max="3" width="33.75" customWidth="1"/>
+    <col min="3" max="3" width="33.7545454545455" customWidth="1"/>
     <col min="4" max="4" width="4.5" customWidth="1"/>
-    <col min="5" max="8" width="33.75" customWidth="1"/>
-    <col min="9" max="9" width="28.25" customWidth="1"/>
+    <col min="5" max="8" width="33.7545454545455" customWidth="1"/>
+    <col min="9" max="9" width="28.2545454545455" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="8:8">
@@ -33759,91 +33621,67 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="8:9">
-      <c r="H3" t="s">
+    <row r="3" spans="9:9">
+      <c r="I3" t="s">
         <v>1</v>
-      </c>
-      <c r="I3" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="4" spans="8:9">
       <c r="H4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="8:9">
-      <c r="H5" t="s">
-        <v>5</v>
-      </c>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="9:9">
       <c r="I5">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H6" t="s">
+        <v>5</v>
+      </c>
+      <c r="I6" t="s">
         <v>6</v>
       </c>
-      <c r="H6" t="s">
+    </row>
+    <row r="7" spans="2:9">
+      <c r="B7" t="s">
         <v>7</v>
       </c>
-      <c r="I6" t="s">
+      <c r="C7" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" t="s">
-        <v>11</v>
       </c>
       <c r="D7">
         <v>301</v>
       </c>
-      <c r="H7" t="s">
-        <v>12</v>
-      </c>
-      <c r="I7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="8:9">
-      <c r="H8" t="s">
-        <v>14</v>
-      </c>
+      <c r="I7">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="8" spans="9:9">
       <c r="I8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H9" t="s">
-        <v>17</v>
-      </c>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="9:9">
       <c r="I9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="8:9">
-      <c r="H10" t="s">
-        <v>19</v>
-      </c>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="9:9">
       <c r="I10" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="8:9">
       <c r="H11" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="I11">
         <v>301</v>
@@ -33851,39 +33689,39 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="E15" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="F15" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="G15" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="H15" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="C16" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="E16" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="F16" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="G16" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="H16" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -39918,18 +39756,18 @@
   <sheetPr/>
   <dimension ref="A1:I377"/>
   <sheetViews>
-    <sheetView topLeftCell="A349" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17:C377"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="58.25" customWidth="1"/>
+    <col min="1" max="1" width="58.2545454545455" customWidth="1"/>
     <col min="2" max="2" width="7.5" customWidth="1"/>
     <col min="3" max="3" width="31.5" customWidth="1"/>
     <col min="4" max="4" width="4.5" customWidth="1"/>
     <col min="5" max="8" width="31.5" customWidth="1"/>
-    <col min="9" max="9" width="28.25" customWidth="1"/>
+    <col min="9" max="9" width="28.2545454545455" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="8:8">
@@ -39937,91 +39775,67 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="8:9">
-      <c r="H3" t="s">
+    <row r="3" spans="9:9">
+      <c r="I3" t="s">
         <v>1</v>
-      </c>
-      <c r="I3" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="4" spans="8:9">
       <c r="H4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="8:9">
-      <c r="H5" t="s">
-        <v>5</v>
-      </c>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="9:9">
       <c r="I5">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H6" t="s">
+        <v>5</v>
+      </c>
+      <c r="I6" t="s">
         <v>6</v>
       </c>
-      <c r="H6" t="s">
+    </row>
+    <row r="7" spans="2:9">
+      <c r="B7" t="s">
         <v>7</v>
       </c>
-      <c r="I6" t="s">
+      <c r="C7" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" t="s">
-        <v>11</v>
       </c>
       <c r="D7">
         <v>361</v>
       </c>
-      <c r="H7" t="s">
-        <v>12</v>
-      </c>
-      <c r="I7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="8:9">
-      <c r="H8" t="s">
-        <v>14</v>
-      </c>
+      <c r="I7">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="8" spans="9:9">
       <c r="I8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" t="s">
-        <v>44</v>
-      </c>
-      <c r="H9" t="s">
-        <v>17</v>
-      </c>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="9:9">
       <c r="I9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="8:9">
-      <c r="H10" t="s">
-        <v>19</v>
-      </c>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="9:9">
       <c r="I10" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="8:9">
       <c r="H11" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="I11">
         <v>361</v>
@@ -40029,39 +39843,39 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="E15" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="F15" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="G15" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="H15" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="C16" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="E16" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="F16" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="G16" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="H16" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -47289,3047 +47103,4 @@
   <headerFooter/>
   <drawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:D12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="3"/>
-  <cols>
-    <col min="1" max="1" width="41.6296296296296" customWidth="1"/>
-    <col min="2" max="2" width="10.5" customWidth="1"/>
-    <col min="3" max="3" width="59.3796296296296" customWidth="1"/>
-    <col min="4" max="4" width="5.25" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1">
-      <c r="A5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" t="s">
-        <v>49</v>
-      </c>
-      <c r="B7" t="s">
-        <v>50</v>
-      </c>
-      <c r="C7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D7" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3">
-      <c r="B8" t="s">
-        <v>53</v>
-      </c>
-      <c r="C8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3">
-      <c r="B9" t="s">
-        <v>54</v>
-      </c>
-      <c r="C9" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" spans="2:3">
-      <c r="B10" t="s">
-        <v>55</v>
-      </c>
-      <c r="C10" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="2:3">
-      <c r="B11" t="s">
-        <v>56</v>
-      </c>
-      <c r="C11" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="2:3">
-      <c r="B12" t="s">
-        <v>57</v>
-      </c>
-      <c r="C12" t="s">
-        <v>44</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:B362"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B362"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="1"/>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2">
-        <v>392.5</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3">
-        <v>392.55</v>
-      </c>
-      <c r="B3">
-        <v>5072.17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4">
-        <v>392.6</v>
-      </c>
-      <c r="B4">
-        <v>5072.17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5">
-        <v>392.65</v>
-      </c>
-      <c r="B5">
-        <v>5072.17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6">
-        <v>392.7</v>
-      </c>
-      <c r="B6">
-        <v>5072.17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7">
-        <v>392.75</v>
-      </c>
-      <c r="B7">
-        <v>5072.17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8">
-        <v>392.8</v>
-      </c>
-      <c r="B8">
-        <v>5072.17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9">
-        <v>392.85</v>
-      </c>
-      <c r="B9">
-        <v>5072.17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10">
-        <v>392.9</v>
-      </c>
-      <c r="B10">
-        <v>5072.17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11">
-        <v>392.95</v>
-      </c>
-      <c r="B11">
-        <v>5072.19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12">
-        <v>393</v>
-      </c>
-      <c r="B12">
-        <v>5072.23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13">
-        <v>393.05</v>
-      </c>
-      <c r="B13">
-        <v>5072.28</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14">
-        <v>393.1</v>
-      </c>
-      <c r="B14">
-        <v>5072.33</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15">
-        <v>393.15</v>
-      </c>
-      <c r="B15">
-        <v>5072.38</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16">
-        <v>393.2</v>
-      </c>
-      <c r="B16">
-        <v>5072.42</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17">
-        <v>393.25</v>
-      </c>
-      <c r="B17">
-        <v>5072.46</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18">
-        <v>393.3</v>
-      </c>
-      <c r="B18">
-        <v>5072.5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19">
-        <v>393.35</v>
-      </c>
-      <c r="B19">
-        <v>5072.54</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20">
-        <v>393.4</v>
-      </c>
-      <c r="B20">
-        <v>5072.57</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21">
-        <v>393.45</v>
-      </c>
-      <c r="B21">
-        <v>5072.6</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22">
-        <v>393.5</v>
-      </c>
-      <c r="B22">
-        <v>5072.61</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23">
-        <v>393.55</v>
-      </c>
-      <c r="B23">
-        <v>5072.61</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24">
-        <v>393.6</v>
-      </c>
-      <c r="B24">
-        <v>5072.61</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25">
-        <v>393.65</v>
-      </c>
-      <c r="B25">
-        <v>5072.62</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26">
-        <v>393.7</v>
-      </c>
-      <c r="B26">
-        <v>5072.66</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2">
-      <c r="A27">
-        <v>393.75</v>
-      </c>
-      <c r="B27">
-        <v>5072.72</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2">
-      <c r="A28">
-        <v>393.8</v>
-      </c>
-      <c r="B28">
-        <v>5072.77</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2">
-      <c r="A29">
-        <v>393.85</v>
-      </c>
-      <c r="B29">
-        <v>5072.83</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2">
-      <c r="A30">
-        <v>393.9</v>
-      </c>
-      <c r="B30">
-        <v>5072.9</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2">
-      <c r="A31">
-        <v>393.95</v>
-      </c>
-      <c r="B31">
-        <v>5072.97</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2">
-      <c r="A32">
-        <v>394</v>
-      </c>
-      <c r="B32">
-        <v>5073.05</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2">
-      <c r="A33">
-        <v>394.05</v>
-      </c>
-      <c r="B33">
-        <v>5073.12</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2">
-      <c r="A34">
-        <v>394.1</v>
-      </c>
-      <c r="B34">
-        <v>5073.17</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2">
-      <c r="A35">
-        <v>394.15</v>
-      </c>
-      <c r="B35">
-        <v>5073.23</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2">
-      <c r="A36">
-        <v>394.2</v>
-      </c>
-      <c r="B36">
-        <v>5073.28</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2">
-      <c r="A37">
-        <v>394.25</v>
-      </c>
-      <c r="B37">
-        <v>5073.34</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2">
-      <c r="A38">
-        <v>394.3</v>
-      </c>
-      <c r="B38">
-        <v>5073.41</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2">
-      <c r="A39">
-        <v>394.35</v>
-      </c>
-      <c r="B39">
-        <v>5073.5</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2">
-      <c r="A40">
-        <v>394.4</v>
-      </c>
-      <c r="B40">
-        <v>5073.62</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2">
-      <c r="A41">
-        <v>394.45</v>
-      </c>
-      <c r="B41">
-        <v>5073.74</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2">
-      <c r="A42">
-        <v>394.5</v>
-      </c>
-      <c r="B42">
-        <v>5073.89</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2">
-      <c r="A43">
-        <v>394.55</v>
-      </c>
-      <c r="B43">
-        <v>5074.06</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2">
-      <c r="A44">
-        <v>394.6</v>
-      </c>
-      <c r="B44">
-        <v>5074.23</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2">
-      <c r="A45">
-        <v>394.65</v>
-      </c>
-      <c r="B45">
-        <v>5074.41</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2">
-      <c r="A46">
-        <v>394.7</v>
-      </c>
-      <c r="B46">
-        <v>5074.57</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2">
-      <c r="A47">
-        <v>394.75</v>
-      </c>
-      <c r="B47">
-        <v>5074.72</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2">
-      <c r="A48">
-        <v>394.8</v>
-      </c>
-      <c r="B48">
-        <v>5074.87</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2">
-      <c r="A49">
-        <v>394.85</v>
-      </c>
-      <c r="B49">
-        <v>5075</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2">
-      <c r="A50">
-        <v>394.9</v>
-      </c>
-      <c r="B50">
-        <v>5075.1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2">
-      <c r="A51">
-        <v>394.95</v>
-      </c>
-      <c r="B51">
-        <v>5075.2</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2">
-      <c r="A52">
-        <v>395</v>
-      </c>
-      <c r="B52">
-        <v>5075.29</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2">
-      <c r="A53">
-        <v>395.05</v>
-      </c>
-      <c r="B53">
-        <v>5075.36</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2">
-      <c r="A54">
-        <v>395.1</v>
-      </c>
-      <c r="B54">
-        <v>5075.42</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2">
-      <c r="A55">
-        <v>395.15</v>
-      </c>
-      <c r="B55">
-        <v>5075.48</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2">
-      <c r="A56">
-        <v>395.2</v>
-      </c>
-      <c r="B56">
-        <v>5075.56</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2">
-      <c r="A57">
-        <v>395.25</v>
-      </c>
-      <c r="B57">
-        <v>5075.65</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2">
-      <c r="A58">
-        <v>395.3</v>
-      </c>
-      <c r="B58">
-        <v>5075.75</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2">
-      <c r="A59">
-        <v>395.35</v>
-      </c>
-      <c r="B59">
-        <v>5075.83</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2">
-      <c r="A60">
-        <v>395.4</v>
-      </c>
-      <c r="B60">
-        <v>5075.9</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2">
-      <c r="A61">
-        <v>395.45</v>
-      </c>
-      <c r="B61">
-        <v>5075.94</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2">
-      <c r="A62">
-        <v>395.5</v>
-      </c>
-      <c r="B62">
-        <v>5075.98</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2">
-      <c r="A63">
-        <v>395.55</v>
-      </c>
-      <c r="B63">
-        <v>5076.01</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2">
-      <c r="A64">
-        <v>395.6</v>
-      </c>
-      <c r="B64">
-        <v>5076.05</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2">
-      <c r="A65">
-        <v>395.65</v>
-      </c>
-      <c r="B65">
-        <v>5076.13</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2">
-      <c r="A66">
-        <v>395.7</v>
-      </c>
-      <c r="B66">
-        <v>5076.23</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2">
-      <c r="A67">
-        <v>395.75</v>
-      </c>
-      <c r="B67">
-        <v>5076.32</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2">
-      <c r="A68">
-        <v>395.8</v>
-      </c>
-      <c r="B68">
-        <v>5076.4</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2">
-      <c r="A69">
-        <v>395.85</v>
-      </c>
-      <c r="B69">
-        <v>5076.49</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2">
-      <c r="A70">
-        <v>395.9</v>
-      </c>
-      <c r="B70">
-        <v>5076.58</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2">
-      <c r="A71">
-        <v>395.95</v>
-      </c>
-      <c r="B71">
-        <v>5076.71</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2">
-      <c r="A72">
-        <v>396</v>
-      </c>
-      <c r="B72">
-        <v>5076.86</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2">
-      <c r="A73">
-        <v>396.05</v>
-      </c>
-      <c r="B73">
-        <v>5077</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2">
-      <c r="A74">
-        <v>396.1</v>
-      </c>
-      <c r="B74">
-        <v>5077.15</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2">
-      <c r="A75">
-        <v>396.15</v>
-      </c>
-      <c r="B75">
-        <v>5077.28</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2">
-      <c r="A76">
-        <v>396.2</v>
-      </c>
-      <c r="B76">
-        <v>5077.4</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2">
-      <c r="A77">
-        <v>396.25</v>
-      </c>
-      <c r="B77">
-        <v>5077.51</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2">
-      <c r="A78">
-        <v>396.3</v>
-      </c>
-      <c r="B78">
-        <v>5077.6</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2">
-      <c r="A79">
-        <v>396.35</v>
-      </c>
-      <c r="B79">
-        <v>5077.7</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2">
-      <c r="A80">
-        <v>396.4</v>
-      </c>
-      <c r="B80">
-        <v>5077.8</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2">
-      <c r="A81">
-        <v>396.45</v>
-      </c>
-      <c r="B81">
-        <v>5077.92</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2">
-      <c r="A82">
-        <v>396.5</v>
-      </c>
-      <c r="B82">
-        <v>5078.04</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2">
-      <c r="A83">
-        <v>396.55</v>
-      </c>
-      <c r="B83">
-        <v>5078.14</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2">
-      <c r="A84">
-        <v>396.6</v>
-      </c>
-      <c r="B84">
-        <v>5078.24</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2">
-      <c r="A85">
-        <v>396.65</v>
-      </c>
-      <c r="B85">
-        <v>5078.34</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2">
-      <c r="A86">
-        <v>396.7</v>
-      </c>
-      <c r="B86">
-        <v>5078.42</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2">
-      <c r="A87">
-        <v>396.75</v>
-      </c>
-      <c r="B87">
-        <v>5078.49</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2">
-      <c r="A88">
-        <v>396.8</v>
-      </c>
-      <c r="B88">
-        <v>5078.57</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2">
-      <c r="A89">
-        <v>396.85</v>
-      </c>
-      <c r="B89">
-        <v>5078.66</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2">
-      <c r="A90">
-        <v>396.9</v>
-      </c>
-      <c r="B90">
-        <v>5078.77</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2">
-      <c r="A91">
-        <v>396.95</v>
-      </c>
-      <c r="B91">
-        <v>5078.86</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2">
-      <c r="A92">
-        <v>397</v>
-      </c>
-      <c r="B92">
-        <v>5078.93</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2">
-      <c r="A93">
-        <v>397.05</v>
-      </c>
-      <c r="B93">
-        <v>5078.99</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2">
-      <c r="A94">
-        <v>397.1</v>
-      </c>
-      <c r="B94">
-        <v>5079.05</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2">
-      <c r="A95">
-        <v>397.15</v>
-      </c>
-      <c r="B95">
-        <v>5079.11</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2">
-      <c r="A96">
-        <v>397.2</v>
-      </c>
-      <c r="B96">
-        <v>5079.17</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2">
-      <c r="A97">
-        <v>397.25</v>
-      </c>
-      <c r="B97">
-        <v>5079.25</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2">
-      <c r="A98">
-        <v>397.3</v>
-      </c>
-      <c r="B98">
-        <v>5079.34</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2">
-      <c r="A99">
-        <v>397.35</v>
-      </c>
-      <c r="B99">
-        <v>5079.44</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2">
-      <c r="A100">
-        <v>397.4</v>
-      </c>
-      <c r="B100">
-        <v>5079.53</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2">
-      <c r="A101">
-        <v>397.45</v>
-      </c>
-      <c r="B101">
-        <v>5079.61</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2">
-      <c r="A102">
-        <v>397.5</v>
-      </c>
-      <c r="B102">
-        <v>5079.71</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2">
-      <c r="A103">
-        <v>397.55</v>
-      </c>
-      <c r="B103">
-        <v>5079.8</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2">
-      <c r="A104">
-        <v>397.6</v>
-      </c>
-      <c r="B104">
-        <v>5079.91</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2">
-      <c r="A105">
-        <v>397.65</v>
-      </c>
-      <c r="B105">
-        <v>5080.05</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2">
-      <c r="A106">
-        <v>397.7</v>
-      </c>
-      <c r="B106">
-        <v>5080.19</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2">
-      <c r="A107">
-        <v>397.75</v>
-      </c>
-      <c r="B107">
-        <v>5080.34</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2">
-      <c r="A108">
-        <v>397.8</v>
-      </c>
-      <c r="B108">
-        <v>5080.49</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2">
-      <c r="A109">
-        <v>397.85</v>
-      </c>
-      <c r="B109">
-        <v>5080.63</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2">
-      <c r="A110">
-        <v>397.9</v>
-      </c>
-      <c r="B110">
-        <v>5080.76</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2">
-      <c r="A111">
-        <v>397.95</v>
-      </c>
-      <c r="B111">
-        <v>5080.87</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2">
-      <c r="A112">
-        <v>398</v>
-      </c>
-      <c r="B112">
-        <v>5080.98</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2">
-      <c r="A113">
-        <v>398.05</v>
-      </c>
-      <c r="B113">
-        <v>5081.07</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2">
-      <c r="A114">
-        <v>398.1</v>
-      </c>
-      <c r="B114">
-        <v>5081.19</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2">
-      <c r="A115">
-        <v>398.15</v>
-      </c>
-      <c r="B115">
-        <v>5081.32</v>
-      </c>
-    </row>
-    <row r="116" spans="1:2">
-      <c r="A116">
-        <v>398.2</v>
-      </c>
-      <c r="B116">
-        <v>5081.44</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2">
-      <c r="A117">
-        <v>398.25</v>
-      </c>
-      <c r="B117">
-        <v>5081.56</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2">
-      <c r="A118">
-        <v>398.3</v>
-      </c>
-      <c r="B118">
-        <v>5081.7</v>
-      </c>
-    </row>
-    <row r="119" spans="1:2">
-      <c r="A119">
-        <v>398.35</v>
-      </c>
-      <c r="B119">
-        <v>5081.83</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2">
-      <c r="A120">
-        <v>398.4</v>
-      </c>
-      <c r="B120">
-        <v>5081.97</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2">
-      <c r="A121">
-        <v>398.45</v>
-      </c>
-      <c r="B121">
-        <v>5082.14</v>
-      </c>
-    </row>
-    <row r="122" spans="1:2">
-      <c r="A122">
-        <v>398.5</v>
-      </c>
-      <c r="B122">
-        <v>5082.33</v>
-      </c>
-    </row>
-    <row r="123" spans="1:2">
-      <c r="A123">
-        <v>398.55</v>
-      </c>
-      <c r="B123">
-        <v>5082.57</v>
-      </c>
-    </row>
-    <row r="124" spans="1:2">
-      <c r="A124">
-        <v>398.6</v>
-      </c>
-      <c r="B124">
-        <v>5082.82</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2">
-      <c r="A125">
-        <v>398.65</v>
-      </c>
-      <c r="B125">
-        <v>5083.08</v>
-      </c>
-    </row>
-    <row r="126" spans="1:2">
-      <c r="A126">
-        <v>398.7</v>
-      </c>
-      <c r="B126">
-        <v>5083.34</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2">
-      <c r="A127">
-        <v>398.75</v>
-      </c>
-      <c r="B127">
-        <v>5083.6</v>
-      </c>
-    </row>
-    <row r="128" spans="1:2">
-      <c r="A128">
-        <v>398.8</v>
-      </c>
-      <c r="B128">
-        <v>5083.89</v>
-      </c>
-    </row>
-    <row r="129" spans="1:2">
-      <c r="A129">
-        <v>398.85</v>
-      </c>
-      <c r="B129">
-        <v>5084.19</v>
-      </c>
-    </row>
-    <row r="130" spans="1:2">
-      <c r="A130">
-        <v>398.9</v>
-      </c>
-      <c r="B130">
-        <v>5084.53</v>
-      </c>
-    </row>
-    <row r="131" spans="1:2">
-      <c r="A131">
-        <v>398.95</v>
-      </c>
-      <c r="B131">
-        <v>5084.91</v>
-      </c>
-    </row>
-    <row r="132" spans="1:2">
-      <c r="A132">
-        <v>399</v>
-      </c>
-      <c r="B132">
-        <v>5085.29</v>
-      </c>
-    </row>
-    <row r="133" spans="1:2">
-      <c r="A133">
-        <v>399.05</v>
-      </c>
-      <c r="B133">
-        <v>5085.68</v>
-      </c>
-    </row>
-    <row r="134" spans="1:2">
-      <c r="A134">
-        <v>399.1</v>
-      </c>
-      <c r="B134">
-        <v>5086.05</v>
-      </c>
-    </row>
-    <row r="135" spans="1:2">
-      <c r="A135">
-        <v>399.15</v>
-      </c>
-      <c r="B135">
-        <v>5086.47</v>
-      </c>
-    </row>
-    <row r="136" spans="1:2">
-      <c r="A136">
-        <v>399.2</v>
-      </c>
-      <c r="B136">
-        <v>5086.93</v>
-      </c>
-    </row>
-    <row r="137" spans="1:2">
-      <c r="A137">
-        <v>399.25</v>
-      </c>
-      <c r="B137">
-        <v>5087.42</v>
-      </c>
-    </row>
-    <row r="138" spans="1:2">
-      <c r="A138">
-        <v>399.3</v>
-      </c>
-      <c r="B138">
-        <v>5087.94</v>
-      </c>
-    </row>
-    <row r="139" spans="1:2">
-      <c r="A139">
-        <v>399.35</v>
-      </c>
-      <c r="B139">
-        <v>5088.5</v>
-      </c>
-    </row>
-    <row r="140" spans="1:2">
-      <c r="A140">
-        <v>399.4</v>
-      </c>
-      <c r="B140">
-        <v>5089.12</v>
-      </c>
-    </row>
-    <row r="141" spans="1:2">
-      <c r="A141">
-        <v>399.45</v>
-      </c>
-      <c r="B141">
-        <v>5089.82</v>
-      </c>
-    </row>
-    <row r="142" spans="1:2">
-      <c r="A142">
-        <v>399.5</v>
-      </c>
-      <c r="B142">
-        <v>5090.63</v>
-      </c>
-    </row>
-    <row r="143" spans="1:2">
-      <c r="A143">
-        <v>399.55</v>
-      </c>
-      <c r="B143">
-        <v>5091.58</v>
-      </c>
-    </row>
-    <row r="144" spans="1:2">
-      <c r="A144">
-        <v>399.6</v>
-      </c>
-      <c r="B144">
-        <v>5092.76</v>
-      </c>
-    </row>
-    <row r="145" spans="1:2">
-      <c r="A145">
-        <v>399.65</v>
-      </c>
-      <c r="B145">
-        <v>5094.21</v>
-      </c>
-    </row>
-    <row r="146" spans="1:2">
-      <c r="A146">
-        <v>399.7</v>
-      </c>
-      <c r="B146">
-        <v>5095.95</v>
-      </c>
-    </row>
-    <row r="147" spans="1:2">
-      <c r="A147">
-        <v>399.75</v>
-      </c>
-      <c r="B147">
-        <v>5098.07</v>
-      </c>
-    </row>
-    <row r="148" spans="1:2">
-      <c r="A148">
-        <v>399.8</v>
-      </c>
-      <c r="B148">
-        <v>5100.65</v>
-      </c>
-    </row>
-    <row r="149" spans="1:2">
-      <c r="A149">
-        <v>399.85</v>
-      </c>
-      <c r="B149">
-        <v>5103.79</v>
-      </c>
-    </row>
-    <row r="150" spans="1:2">
-      <c r="A150">
-        <v>399.9</v>
-      </c>
-      <c r="B150">
-        <v>5107.58</v>
-      </c>
-    </row>
-    <row r="151" spans="1:2">
-      <c r="A151">
-        <v>399.95</v>
-      </c>
-      <c r="B151">
-        <v>5112.04</v>
-      </c>
-    </row>
-    <row r="152" spans="1:2">
-      <c r="A152">
-        <v>400</v>
-      </c>
-      <c r="B152">
-        <v>5117.24</v>
-      </c>
-    </row>
-    <row r="153" spans="1:2">
-      <c r="A153">
-        <v>400.05</v>
-      </c>
-      <c r="B153">
-        <v>5123.27</v>
-      </c>
-    </row>
-    <row r="154" spans="1:2">
-      <c r="A154">
-        <v>400.1</v>
-      </c>
-      <c r="B154">
-        <v>5130.16</v>
-      </c>
-    </row>
-    <row r="155" spans="1:2">
-      <c r="A155">
-        <v>400.15</v>
-      </c>
-      <c r="B155">
-        <v>5137.92</v>
-      </c>
-    </row>
-    <row r="156" spans="1:2">
-      <c r="A156">
-        <v>400.2</v>
-      </c>
-      <c r="B156">
-        <v>5146.56</v>
-      </c>
-    </row>
-    <row r="157" spans="1:2">
-      <c r="A157">
-        <v>400.25</v>
-      </c>
-      <c r="B157">
-        <v>5156.03</v>
-      </c>
-    </row>
-    <row r="158" spans="1:2">
-      <c r="A158">
-        <v>400.3</v>
-      </c>
-      <c r="B158">
-        <v>5166.27</v>
-      </c>
-    </row>
-    <row r="159" spans="1:2">
-      <c r="A159">
-        <v>400.35</v>
-      </c>
-      <c r="B159">
-        <v>5177.18</v>
-      </c>
-    </row>
-    <row r="160" spans="1:2">
-      <c r="A160">
-        <v>400.4</v>
-      </c>
-      <c r="B160">
-        <v>5188.66</v>
-      </c>
-    </row>
-    <row r="161" spans="1:2">
-      <c r="A161">
-        <v>400.45</v>
-      </c>
-      <c r="B161">
-        <v>5200.54</v>
-      </c>
-    </row>
-    <row r="162" spans="1:2">
-      <c r="A162">
-        <v>400.5</v>
-      </c>
-      <c r="B162">
-        <v>5212.72</v>
-      </c>
-    </row>
-    <row r="163" spans="1:2">
-      <c r="A163">
-        <v>400.55</v>
-      </c>
-      <c r="B163">
-        <v>5225.07</v>
-      </c>
-    </row>
-    <row r="164" spans="1:2">
-      <c r="A164">
-        <v>400.6</v>
-      </c>
-      <c r="B164">
-        <v>5237.39</v>
-      </c>
-    </row>
-    <row r="165" spans="1:2">
-      <c r="A165">
-        <v>400.65</v>
-      </c>
-      <c r="B165">
-        <v>5249.53</v>
-      </c>
-    </row>
-    <row r="166" spans="1:2">
-      <c r="A166">
-        <v>400.7</v>
-      </c>
-      <c r="B166">
-        <v>5261.34</v>
-      </c>
-    </row>
-    <row r="167" spans="1:2">
-      <c r="A167">
-        <v>400.75</v>
-      </c>
-      <c r="B167">
-        <v>5272.72</v>
-      </c>
-    </row>
-    <row r="168" spans="1:2">
-      <c r="A168">
-        <v>400.8</v>
-      </c>
-      <c r="B168">
-        <v>5283.57</v>
-      </c>
-    </row>
-    <row r="169" spans="1:2">
-      <c r="A169">
-        <v>400.85</v>
-      </c>
-      <c r="B169">
-        <v>5293.81</v>
-      </c>
-    </row>
-    <row r="170" spans="1:2">
-      <c r="A170">
-        <v>400.9</v>
-      </c>
-      <c r="B170">
-        <v>5303.34</v>
-      </c>
-    </row>
-    <row r="171" spans="1:2">
-      <c r="A171">
-        <v>400.95</v>
-      </c>
-      <c r="B171">
-        <v>5312.09</v>
-      </c>
-    </row>
-    <row r="172" spans="1:2">
-      <c r="A172">
-        <v>401</v>
-      </c>
-      <c r="B172">
-        <v>5320.1</v>
-      </c>
-    </row>
-    <row r="173" spans="1:2">
-      <c r="A173">
-        <v>401.05</v>
-      </c>
-      <c r="B173">
-        <v>5327.36</v>
-      </c>
-    </row>
-    <row r="174" spans="1:2">
-      <c r="A174">
-        <v>401.1</v>
-      </c>
-      <c r="B174">
-        <v>5333.87</v>
-      </c>
-    </row>
-    <row r="175" spans="1:2">
-      <c r="A175">
-        <v>401.15</v>
-      </c>
-      <c r="B175">
-        <v>5339.68</v>
-      </c>
-    </row>
-    <row r="176" spans="1:2">
-      <c r="A176">
-        <v>401.2</v>
-      </c>
-      <c r="B176">
-        <v>5344.81</v>
-      </c>
-    </row>
-    <row r="177" spans="1:2">
-      <c r="A177">
-        <v>401.25</v>
-      </c>
-      <c r="B177">
-        <v>5349.31</v>
-      </c>
-    </row>
-    <row r="178" spans="1:2">
-      <c r="A178">
-        <v>401.3</v>
-      </c>
-      <c r="B178">
-        <v>5353.19</v>
-      </c>
-    </row>
-    <row r="179" spans="1:2">
-      <c r="A179">
-        <v>401.35</v>
-      </c>
-      <c r="B179">
-        <v>5356.51</v>
-      </c>
-    </row>
-    <row r="180" spans="1:2">
-      <c r="A180">
-        <v>401.4</v>
-      </c>
-      <c r="B180">
-        <v>5359.34</v>
-      </c>
-    </row>
-    <row r="181" spans="1:2">
-      <c r="A181">
-        <v>401.45</v>
-      </c>
-      <c r="B181">
-        <v>5361.82</v>
-      </c>
-    </row>
-    <row r="182" spans="1:2">
-      <c r="A182">
-        <v>401.5</v>
-      </c>
-      <c r="B182">
-        <v>5363.98</v>
-      </c>
-    </row>
-    <row r="183" spans="1:2">
-      <c r="A183">
-        <v>401.55</v>
-      </c>
-      <c r="B183">
-        <v>5365.83</v>
-      </c>
-    </row>
-    <row r="184" spans="1:2">
-      <c r="A184">
-        <v>401.6</v>
-      </c>
-      <c r="B184">
-        <v>5367.4</v>
-      </c>
-    </row>
-    <row r="185" spans="1:2">
-      <c r="A185">
-        <v>401.65</v>
-      </c>
-      <c r="B185">
-        <v>5368.71</v>
-      </c>
-    </row>
-    <row r="186" spans="1:2">
-      <c r="A186">
-        <v>401.7</v>
-      </c>
-      <c r="B186">
-        <v>5369.83</v>
-      </c>
-    </row>
-    <row r="187" spans="1:2">
-      <c r="A187">
-        <v>401.75</v>
-      </c>
-      <c r="B187">
-        <v>5370.8</v>
-      </c>
-    </row>
-    <row r="188" spans="1:2">
-      <c r="A188">
-        <v>401.8</v>
-      </c>
-      <c r="B188">
-        <v>5371.67</v>
-      </c>
-    </row>
-    <row r="189" spans="1:2">
-      <c r="A189">
-        <v>401.85</v>
-      </c>
-      <c r="B189">
-        <v>5372.44</v>
-      </c>
-    </row>
-    <row r="190" spans="1:2">
-      <c r="A190">
-        <v>401.9</v>
-      </c>
-      <c r="B190">
-        <v>5373.13</v>
-      </c>
-    </row>
-    <row r="191" spans="1:2">
-      <c r="A191">
-        <v>401.95</v>
-      </c>
-      <c r="B191">
-        <v>5373.75</v>
-      </c>
-    </row>
-    <row r="192" spans="1:2">
-      <c r="A192">
-        <v>402</v>
-      </c>
-      <c r="B192">
-        <v>5374.29</v>
-      </c>
-    </row>
-    <row r="193" spans="1:2">
-      <c r="A193">
-        <v>402.05</v>
-      </c>
-      <c r="B193">
-        <v>5374.78</v>
-      </c>
-    </row>
-    <row r="194" spans="1:2">
-      <c r="A194">
-        <v>402.1</v>
-      </c>
-      <c r="B194">
-        <v>5375.24</v>
-      </c>
-    </row>
-    <row r="195" spans="1:2">
-      <c r="A195">
-        <v>402.15</v>
-      </c>
-      <c r="B195">
-        <v>5375.68</v>
-      </c>
-    </row>
-    <row r="196" spans="1:2">
-      <c r="A196">
-        <v>402.2</v>
-      </c>
-      <c r="B196">
-        <v>5376.09</v>
-      </c>
-    </row>
-    <row r="197" spans="1:2">
-      <c r="A197">
-        <v>402.25</v>
-      </c>
-      <c r="B197">
-        <v>5376.45</v>
-      </c>
-    </row>
-    <row r="198" spans="1:2">
-      <c r="A198">
-        <v>402.3</v>
-      </c>
-      <c r="B198">
-        <v>5376.77</v>
-      </c>
-    </row>
-    <row r="199" spans="1:2">
-      <c r="A199">
-        <v>402.35</v>
-      </c>
-      <c r="B199">
-        <v>5377.04</v>
-      </c>
-    </row>
-    <row r="200" spans="1:2">
-      <c r="A200">
-        <v>402.4</v>
-      </c>
-      <c r="B200">
-        <v>5377.27</v>
-      </c>
-    </row>
-    <row r="201" spans="1:2">
-      <c r="A201">
-        <v>402.45</v>
-      </c>
-      <c r="B201">
-        <v>5377.5</v>
-      </c>
-    </row>
-    <row r="202" spans="1:2">
-      <c r="A202">
-        <v>402.5</v>
-      </c>
-      <c r="B202">
-        <v>5377.68</v>
-      </c>
-    </row>
-    <row r="203" spans="1:2">
-      <c r="A203">
-        <v>402.55</v>
-      </c>
-      <c r="B203">
-        <v>5377.84</v>
-      </c>
-    </row>
-    <row r="204" spans="1:2">
-      <c r="A204">
-        <v>402.6</v>
-      </c>
-      <c r="B204">
-        <v>5377.97</v>
-      </c>
-    </row>
-    <row r="205" spans="1:2">
-      <c r="A205">
-        <v>402.65</v>
-      </c>
-      <c r="B205">
-        <v>5378.06</v>
-      </c>
-    </row>
-    <row r="206" spans="1:2">
-      <c r="A206">
-        <v>402.7</v>
-      </c>
-      <c r="B206">
-        <v>5378.13</v>
-      </c>
-    </row>
-    <row r="207" spans="1:2">
-      <c r="A207">
-        <v>402.75</v>
-      </c>
-      <c r="B207">
-        <v>5378.21</v>
-      </c>
-    </row>
-    <row r="208" spans="1:2">
-      <c r="A208">
-        <v>402.8</v>
-      </c>
-      <c r="B208">
-        <v>5378.27</v>
-      </c>
-    </row>
-    <row r="209" spans="1:2">
-      <c r="A209">
-        <v>402.85</v>
-      </c>
-      <c r="B209">
-        <v>5378.32</v>
-      </c>
-    </row>
-    <row r="210" spans="1:2">
-      <c r="A210">
-        <v>402.9</v>
-      </c>
-      <c r="B210">
-        <v>5378.89</v>
-      </c>
-    </row>
-    <row r="211" spans="1:2">
-      <c r="A211">
-        <v>402.95</v>
-      </c>
-      <c r="B211">
-        <v>5380.33</v>
-      </c>
-    </row>
-    <row r="212" spans="1:2">
-      <c r="A212">
-        <v>403</v>
-      </c>
-      <c r="B212">
-        <v>5382.14</v>
-      </c>
-    </row>
-    <row r="213" spans="1:2">
-      <c r="A213">
-        <v>403.05</v>
-      </c>
-      <c r="B213">
-        <v>5384.33</v>
-      </c>
-    </row>
-    <row r="214" spans="1:2">
-      <c r="A214">
-        <v>403.1</v>
-      </c>
-      <c r="B214">
-        <v>5386.64</v>
-      </c>
-    </row>
-    <row r="215" spans="1:2">
-      <c r="A215">
-        <v>403.15</v>
-      </c>
-      <c r="B215">
-        <v>5388.49</v>
-      </c>
-    </row>
-    <row r="216" spans="1:2">
-      <c r="A216">
-        <v>403.2</v>
-      </c>
-      <c r="B216">
-        <v>5390.11</v>
-      </c>
-    </row>
-    <row r="217" spans="1:2">
-      <c r="A217">
-        <v>403.25</v>
-      </c>
-      <c r="B217">
-        <v>5391.75</v>
-      </c>
-    </row>
-    <row r="218" spans="1:2">
-      <c r="A218">
-        <v>403.3</v>
-      </c>
-      <c r="B218">
-        <v>5393.76</v>
-      </c>
-    </row>
-    <row r="219" spans="1:2">
-      <c r="A219">
-        <v>403.35</v>
-      </c>
-      <c r="B219">
-        <v>5395.99</v>
-      </c>
-    </row>
-    <row r="220" spans="1:2">
-      <c r="A220">
-        <v>403.4</v>
-      </c>
-      <c r="B220">
-        <v>5398.1</v>
-      </c>
-    </row>
-    <row r="221" spans="1:2">
-      <c r="A221">
-        <v>403.45</v>
-      </c>
-      <c r="B221">
-        <v>5400.38</v>
-      </c>
-    </row>
-    <row r="222" spans="1:2">
-      <c r="A222">
-        <v>403.5</v>
-      </c>
-      <c r="B222">
-        <v>5402.22</v>
-      </c>
-    </row>
-    <row r="223" spans="1:2">
-      <c r="A223">
-        <v>403.55</v>
-      </c>
-      <c r="B223">
-        <v>5403.88</v>
-      </c>
-    </row>
-    <row r="224" spans="1:2">
-      <c r="A224">
-        <v>403.6</v>
-      </c>
-      <c r="B224">
-        <v>5406.79</v>
-      </c>
-    </row>
-    <row r="225" spans="1:2">
-      <c r="A225">
-        <v>403.65</v>
-      </c>
-      <c r="B225">
-        <v>5410.49</v>
-      </c>
-    </row>
-    <row r="226" spans="1:2">
-      <c r="A226">
-        <v>403.7</v>
-      </c>
-      <c r="B226">
-        <v>5415.79</v>
-      </c>
-    </row>
-    <row r="227" spans="1:2">
-      <c r="A227">
-        <v>403.75</v>
-      </c>
-      <c r="B227">
-        <v>5421.65</v>
-      </c>
-    </row>
-    <row r="228" spans="1:2">
-      <c r="A228">
-        <v>403.8</v>
-      </c>
-      <c r="B228">
-        <v>5427.89</v>
-      </c>
-    </row>
-    <row r="229" spans="1:2">
-      <c r="A229">
-        <v>403.85</v>
-      </c>
-      <c r="B229">
-        <v>5434.05</v>
-      </c>
-    </row>
-    <row r="230" spans="1:2">
-      <c r="A230">
-        <v>403.9</v>
-      </c>
-      <c r="B230">
-        <v>5441.26</v>
-      </c>
-    </row>
-    <row r="231" spans="1:2">
-      <c r="A231">
-        <v>403.95</v>
-      </c>
-      <c r="B231">
-        <v>5448.44</v>
-      </c>
-    </row>
-    <row r="232" spans="1:2">
-      <c r="A232">
-        <v>404</v>
-      </c>
-      <c r="B232">
-        <v>5455.03</v>
-      </c>
-    </row>
-    <row r="233" spans="1:2">
-      <c r="A233">
-        <v>404.05</v>
-      </c>
-      <c r="B233">
-        <v>5462.44</v>
-      </c>
-    </row>
-    <row r="234" spans="1:2">
-      <c r="A234">
-        <v>404.1</v>
-      </c>
-      <c r="B234">
-        <v>5469.41</v>
-      </c>
-    </row>
-    <row r="235" spans="1:2">
-      <c r="A235">
-        <v>404.15</v>
-      </c>
-      <c r="B235">
-        <v>5475.31</v>
-      </c>
-    </row>
-    <row r="236" spans="1:2">
-      <c r="A236">
-        <v>404.2</v>
-      </c>
-      <c r="B236">
-        <v>5479.35</v>
-      </c>
-    </row>
-    <row r="237" spans="1:2">
-      <c r="A237">
-        <v>404.25</v>
-      </c>
-      <c r="B237">
-        <v>5481.38</v>
-      </c>
-    </row>
-    <row r="238" spans="1:2">
-      <c r="A238">
-        <v>404.3</v>
-      </c>
-      <c r="B238">
-        <v>5482.76</v>
-      </c>
-    </row>
-    <row r="239" spans="1:2">
-      <c r="A239">
-        <v>404.35</v>
-      </c>
-      <c r="B239">
-        <v>5483.37</v>
-      </c>
-    </row>
-    <row r="240" spans="1:2">
-      <c r="A240">
-        <v>404.4</v>
-      </c>
-      <c r="B240">
-        <v>5483.74</v>
-      </c>
-    </row>
-    <row r="241" spans="1:2">
-      <c r="A241">
-        <v>404.45</v>
-      </c>
-      <c r="B241">
-        <v>5485.36</v>
-      </c>
-    </row>
-    <row r="242" spans="1:2">
-      <c r="A242">
-        <v>404.5</v>
-      </c>
-      <c r="B242">
-        <v>5488.54</v>
-      </c>
-    </row>
-    <row r="243" spans="1:2">
-      <c r="A243">
-        <v>404.55</v>
-      </c>
-      <c r="B243">
-        <v>5491.9</v>
-      </c>
-    </row>
-    <row r="244" spans="1:2">
-      <c r="A244">
-        <v>404.6</v>
-      </c>
-      <c r="B244">
-        <v>5493.73</v>
-      </c>
-    </row>
-    <row r="245" spans="1:2">
-      <c r="A245">
-        <v>404.65</v>
-      </c>
-      <c r="B245">
-        <v>5496.79</v>
-      </c>
-    </row>
-    <row r="246" spans="1:2">
-      <c r="A246">
-        <v>404.7</v>
-      </c>
-      <c r="B246">
-        <v>5500.71</v>
-      </c>
-    </row>
-    <row r="247" spans="1:2">
-      <c r="A247">
-        <v>404.75</v>
-      </c>
-      <c r="B247">
-        <v>5504.7</v>
-      </c>
-    </row>
-    <row r="248" spans="1:2">
-      <c r="A248">
-        <v>404.8</v>
-      </c>
-      <c r="B248">
-        <v>5508.72</v>
-      </c>
-    </row>
-    <row r="249" spans="1:2">
-      <c r="A249">
-        <v>404.85</v>
-      </c>
-      <c r="B249">
-        <v>5513.46</v>
-      </c>
-    </row>
-    <row r="250" spans="1:2">
-      <c r="A250">
-        <v>404.9</v>
-      </c>
-      <c r="B250">
-        <v>5518.83</v>
-      </c>
-    </row>
-    <row r="251" spans="1:2">
-      <c r="A251">
-        <v>404.95</v>
-      </c>
-      <c r="B251">
-        <v>5522.82</v>
-      </c>
-    </row>
-    <row r="252" spans="1:2">
-      <c r="A252">
-        <v>405</v>
-      </c>
-      <c r="B252">
-        <v>5523.61</v>
-      </c>
-    </row>
-    <row r="253" spans="1:2">
-      <c r="A253">
-        <v>405.05</v>
-      </c>
-      <c r="B253">
-        <v>5523.85</v>
-      </c>
-    </row>
-    <row r="254" spans="1:2">
-      <c r="A254">
-        <v>405.1</v>
-      </c>
-      <c r="B254">
-        <v>5529.11</v>
-      </c>
-    </row>
-    <row r="255" spans="1:2">
-      <c r="A255">
-        <v>405.15</v>
-      </c>
-      <c r="B255">
-        <v>5538.88</v>
-      </c>
-    </row>
-    <row r="256" spans="1:2">
-      <c r="A256">
-        <v>405.2</v>
-      </c>
-      <c r="B256">
-        <v>5548.91</v>
-      </c>
-    </row>
-    <row r="257" spans="1:2">
-      <c r="A257">
-        <v>405.25</v>
-      </c>
-      <c r="B257">
-        <v>5552.74</v>
-      </c>
-    </row>
-    <row r="258" spans="1:2">
-      <c r="A258">
-        <v>405.3</v>
-      </c>
-      <c r="B258">
-        <v>5555.81</v>
-      </c>
-    </row>
-    <row r="259" spans="1:2">
-      <c r="A259">
-        <v>405.35</v>
-      </c>
-      <c r="B259">
-        <v>5562.5</v>
-      </c>
-    </row>
-    <row r="260" spans="1:2">
-      <c r="A260">
-        <v>405.4</v>
-      </c>
-      <c r="B260">
-        <v>5571.22</v>
-      </c>
-    </row>
-    <row r="261" spans="1:2">
-      <c r="A261">
-        <v>405.45</v>
-      </c>
-      <c r="B261">
-        <v>5580.79</v>
-      </c>
-    </row>
-    <row r="262" spans="1:2">
-      <c r="A262">
-        <v>405.5</v>
-      </c>
-      <c r="B262">
-        <v>5594.62</v>
-      </c>
-    </row>
-    <row r="263" spans="1:2">
-      <c r="A263">
-        <v>405.55</v>
-      </c>
-      <c r="B263">
-        <v>5611.54</v>
-      </c>
-    </row>
-    <row r="264" spans="1:2">
-      <c r="A264">
-        <v>405.6</v>
-      </c>
-      <c r="B264">
-        <v>5628.61</v>
-      </c>
-    </row>
-    <row r="265" spans="1:2">
-      <c r="A265">
-        <v>405.65</v>
-      </c>
-      <c r="B265">
-        <v>5640.62</v>
-      </c>
-    </row>
-    <row r="266" spans="1:2">
-      <c r="A266">
-        <v>405.7</v>
-      </c>
-      <c r="B266">
-        <v>5646.35</v>
-      </c>
-    </row>
-    <row r="267" spans="1:2">
-      <c r="A267">
-        <v>405.75</v>
-      </c>
-      <c r="B267">
-        <v>5647.39</v>
-      </c>
-    </row>
-    <row r="268" spans="1:2">
-      <c r="A268">
-        <v>405.8</v>
-      </c>
-      <c r="B268">
-        <v>5652.87</v>
-      </c>
-    </row>
-    <row r="269" spans="1:2">
-      <c r="A269">
-        <v>405.85</v>
-      </c>
-      <c r="B269">
-        <v>5661.84</v>
-      </c>
-    </row>
-    <row r="270" spans="1:2">
-      <c r="A270">
-        <v>405.9</v>
-      </c>
-      <c r="B270">
-        <v>5669.39</v>
-      </c>
-    </row>
-    <row r="271" spans="1:2">
-      <c r="A271">
-        <v>405.95</v>
-      </c>
-      <c r="B271">
-        <v>5674.11</v>
-      </c>
-    </row>
-    <row r="272" spans="1:2">
-      <c r="A272">
-        <v>406</v>
-      </c>
-      <c r="B272">
-        <v>5677.37</v>
-      </c>
-    </row>
-    <row r="273" spans="1:2">
-      <c r="A273">
-        <v>406.05</v>
-      </c>
-      <c r="B273">
-        <v>5682.34</v>
-      </c>
-    </row>
-    <row r="274" spans="1:2">
-      <c r="A274">
-        <v>406.1</v>
-      </c>
-      <c r="B274">
-        <v>5689.09</v>
-      </c>
-    </row>
-    <row r="275" spans="1:2">
-      <c r="A275">
-        <v>406.15</v>
-      </c>
-      <c r="B275">
-        <v>5693.96</v>
-      </c>
-    </row>
-    <row r="276" spans="1:2">
-      <c r="A276">
-        <v>406.2</v>
-      </c>
-      <c r="B276">
-        <v>5699.63</v>
-      </c>
-    </row>
-    <row r="277" spans="1:2">
-      <c r="A277">
-        <v>406.25</v>
-      </c>
-      <c r="B277">
-        <v>5708.19</v>
-      </c>
-    </row>
-    <row r="278" spans="1:2">
-      <c r="A278">
-        <v>406.3</v>
-      </c>
-      <c r="B278">
-        <v>5720.32</v>
-      </c>
-    </row>
-    <row r="279" spans="1:2">
-      <c r="A279">
-        <v>406.35</v>
-      </c>
-      <c r="B279">
-        <v>5728.99</v>
-      </c>
-    </row>
-    <row r="280" spans="1:2">
-      <c r="A280">
-        <v>406.4</v>
-      </c>
-      <c r="B280">
-        <v>5734.95</v>
-      </c>
-    </row>
-    <row r="281" spans="1:2">
-      <c r="A281">
-        <v>406.45</v>
-      </c>
-      <c r="B281">
-        <v>5743.85</v>
-      </c>
-    </row>
-    <row r="282" spans="1:2">
-      <c r="A282">
-        <v>406.5</v>
-      </c>
-      <c r="B282">
-        <v>5754.97</v>
-      </c>
-    </row>
-    <row r="283" spans="1:2">
-      <c r="A283">
-        <v>406.55</v>
-      </c>
-      <c r="B283">
-        <v>5767.24</v>
-      </c>
-    </row>
-    <row r="284" spans="1:2">
-      <c r="A284">
-        <v>406.6</v>
-      </c>
-      <c r="B284">
-        <v>5777.65</v>
-      </c>
-    </row>
-    <row r="285" spans="1:2">
-      <c r="A285">
-        <v>406.65</v>
-      </c>
-      <c r="B285">
-        <v>5786.97</v>
-      </c>
-    </row>
-    <row r="286" spans="1:2">
-      <c r="A286">
-        <v>406.7</v>
-      </c>
-      <c r="B286">
-        <v>5794.97</v>
-      </c>
-    </row>
-    <row r="287" spans="1:2">
-      <c r="A287">
-        <v>406.75</v>
-      </c>
-      <c r="B287">
-        <v>5800.31</v>
-      </c>
-    </row>
-    <row r="288" spans="1:2">
-      <c r="A288">
-        <v>406.8</v>
-      </c>
-      <c r="B288">
-        <v>5803.55</v>
-      </c>
-    </row>
-    <row r="289" spans="1:2">
-      <c r="A289">
-        <v>406.85</v>
-      </c>
-      <c r="B289">
-        <v>5804.36</v>
-      </c>
-    </row>
-    <row r="290" spans="1:2">
-      <c r="A290">
-        <v>406.9</v>
-      </c>
-      <c r="B290">
-        <v>5819.68</v>
-      </c>
-    </row>
-    <row r="291" spans="1:2">
-      <c r="A291">
-        <v>406.95</v>
-      </c>
-      <c r="B291">
-        <v>5843.88</v>
-      </c>
-    </row>
-    <row r="292" spans="1:2">
-      <c r="A292">
-        <v>407</v>
-      </c>
-      <c r="B292">
-        <v>5855.47</v>
-      </c>
-    </row>
-    <row r="293" spans="1:2">
-      <c r="A293">
-        <v>407.05</v>
-      </c>
-      <c r="B293">
-        <v>5863.49</v>
-      </c>
-    </row>
-    <row r="294" spans="1:2">
-      <c r="A294">
-        <v>407.1</v>
-      </c>
-      <c r="B294">
-        <v>5879.56</v>
-      </c>
-    </row>
-    <row r="295" spans="1:2">
-      <c r="A295">
-        <v>407.15</v>
-      </c>
-      <c r="B295">
-        <v>5900.55</v>
-      </c>
-    </row>
-    <row r="296" spans="1:2">
-      <c r="A296">
-        <v>407.2</v>
-      </c>
-      <c r="B296">
-        <v>5917.86</v>
-      </c>
-    </row>
-    <row r="297" spans="1:2">
-      <c r="A297">
-        <v>407.25</v>
-      </c>
-      <c r="B297">
-        <v>5943.92</v>
-      </c>
-    </row>
-    <row r="298" spans="1:2">
-      <c r="A298">
-        <v>407.3</v>
-      </c>
-      <c r="B298">
-        <v>5967.34</v>
-      </c>
-    </row>
-    <row r="299" spans="1:2">
-      <c r="A299">
-        <v>407.35</v>
-      </c>
-      <c r="B299">
-        <v>5993.79</v>
-      </c>
-    </row>
-    <row r="300" spans="1:2">
-      <c r="A300">
-        <v>407.4</v>
-      </c>
-      <c r="B300">
-        <v>6012.94</v>
-      </c>
-    </row>
-    <row r="301" spans="1:2">
-      <c r="A301">
-        <v>407.45</v>
-      </c>
-      <c r="B301">
-        <v>6025.24</v>
-      </c>
-    </row>
-    <row r="302" spans="1:2">
-      <c r="A302">
-        <v>407.5</v>
-      </c>
-      <c r="B302">
-        <v>6036.6</v>
-      </c>
-    </row>
-    <row r="303" spans="1:2">
-      <c r="A303">
-        <v>407.55</v>
-      </c>
-      <c r="B303">
-        <v>6051.68</v>
-      </c>
-    </row>
-    <row r="304" spans="1:2">
-      <c r="A304">
-        <v>407.6</v>
-      </c>
-      <c r="B304">
-        <v>6075.88</v>
-      </c>
-    </row>
-    <row r="305" spans="1:2">
-      <c r="A305">
-        <v>407.65</v>
-      </c>
-      <c r="B305">
-        <v>6084.69</v>
-      </c>
-    </row>
-    <row r="306" spans="1:2">
-      <c r="A306">
-        <v>407.7</v>
-      </c>
-      <c r="B306">
-        <v>6087.66</v>
-      </c>
-    </row>
-    <row r="307" spans="1:2">
-      <c r="A307">
-        <v>407.75</v>
-      </c>
-      <c r="B307">
-        <v>6099.84</v>
-      </c>
-    </row>
-    <row r="308" spans="1:2">
-      <c r="A308">
-        <v>407.8</v>
-      </c>
-      <c r="B308">
-        <v>6116.94</v>
-      </c>
-    </row>
-    <row r="309" spans="1:2">
-      <c r="A309">
-        <v>407.85</v>
-      </c>
-      <c r="B309">
-        <v>6130.54</v>
-      </c>
-    </row>
-    <row r="310" spans="1:2">
-      <c r="A310">
-        <v>407.9</v>
-      </c>
-      <c r="B310">
-        <v>6137.4</v>
-      </c>
-    </row>
-    <row r="311" spans="1:2">
-      <c r="A311">
-        <v>407.95</v>
-      </c>
-      <c r="B311">
-        <v>6156.69</v>
-      </c>
-    </row>
-    <row r="312" spans="1:2">
-      <c r="A312">
-        <v>408</v>
-      </c>
-      <c r="B312">
-        <v>6183.4</v>
-      </c>
-    </row>
-    <row r="313" spans="1:2">
-      <c r="A313">
-        <v>408.05</v>
-      </c>
-      <c r="B313">
-        <v>6203.97</v>
-      </c>
-    </row>
-    <row r="314" spans="1:2">
-      <c r="A314">
-        <v>408.1</v>
-      </c>
-      <c r="B314">
-        <v>6221.19</v>
-      </c>
-    </row>
-    <row r="315" spans="1:2">
-      <c r="A315">
-        <v>408.15</v>
-      </c>
-      <c r="B315">
-        <v>6241.92</v>
-      </c>
-    </row>
-    <row r="316" spans="1:2">
-      <c r="A316">
-        <v>408.2</v>
-      </c>
-      <c r="B316">
-        <v>6269.84</v>
-      </c>
-    </row>
-    <row r="317" spans="1:2">
-      <c r="A317">
-        <v>408.25</v>
-      </c>
-      <c r="B317">
-        <v>6298.2</v>
-      </c>
-    </row>
-    <row r="318" spans="1:2">
-      <c r="A318">
-        <v>408.3</v>
-      </c>
-      <c r="B318">
-        <v>6317.75</v>
-      </c>
-    </row>
-    <row r="319" spans="1:2">
-      <c r="A319">
-        <v>408.35</v>
-      </c>
-      <c r="B319">
-        <v>6342.85</v>
-      </c>
-    </row>
-    <row r="320" spans="1:2">
-      <c r="A320">
-        <v>408.4</v>
-      </c>
-      <c r="B320">
-        <v>6370.88</v>
-      </c>
-    </row>
-    <row r="321" spans="1:2">
-      <c r="A321">
-        <v>408.45</v>
-      </c>
-      <c r="B321">
-        <v>6399.09</v>
-      </c>
-    </row>
-    <row r="322" spans="1:2">
-      <c r="A322">
-        <v>408.5</v>
-      </c>
-      <c r="B322">
-        <v>6421.25</v>
-      </c>
-    </row>
-    <row r="323" spans="1:2">
-      <c r="A323">
-        <v>408.55</v>
-      </c>
-      <c r="B323">
-        <v>6428.56</v>
-      </c>
-    </row>
-    <row r="324" spans="1:2">
-      <c r="A324">
-        <v>408.6</v>
-      </c>
-      <c r="B324">
-        <v>6444.39</v>
-      </c>
-    </row>
-    <row r="325" spans="1:2">
-      <c r="A325">
-        <v>408.65</v>
-      </c>
-      <c r="B325">
-        <v>6465.73</v>
-      </c>
-    </row>
-    <row r="326" spans="1:2">
-      <c r="A326">
-        <v>408.7</v>
-      </c>
-      <c r="B326">
-        <v>6487.23</v>
-      </c>
-    </row>
-    <row r="327" spans="1:2">
-      <c r="A327">
-        <v>408.75</v>
-      </c>
-      <c r="B327">
-        <v>6518.09</v>
-      </c>
-    </row>
-    <row r="328" spans="1:2">
-      <c r="A328">
-        <v>408.8</v>
-      </c>
-      <c r="B328">
-        <v>6553.13</v>
-      </c>
-    </row>
-    <row r="329" spans="1:2">
-      <c r="A329">
-        <v>408.85</v>
-      </c>
-      <c r="B329">
-        <v>6581.12</v>
-      </c>
-    </row>
-    <row r="330" spans="1:2">
-      <c r="A330">
-        <v>408.9</v>
-      </c>
-      <c r="B330">
-        <v>6591.19</v>
-      </c>
-    </row>
-    <row r="331" spans="1:2">
-      <c r="A331">
-        <v>408.95</v>
-      </c>
-      <c r="B331">
-        <v>6616.72</v>
-      </c>
-    </row>
-    <row r="332" spans="1:2">
-      <c r="A332">
-        <v>409</v>
-      </c>
-      <c r="B332">
-        <v>6640.12</v>
-      </c>
-    </row>
-    <row r="333" spans="1:2">
-      <c r="A333">
-        <v>409.05</v>
-      </c>
-      <c r="B333">
-        <v>6668.84</v>
-      </c>
-    </row>
-    <row r="334" spans="1:2">
-      <c r="A334">
-        <v>409.1</v>
-      </c>
-      <c r="B334">
-        <v>6706.92</v>
-      </c>
-    </row>
-    <row r="335" spans="1:2">
-      <c r="A335">
-        <v>409.15</v>
-      </c>
-      <c r="B335">
-        <v>6736.82</v>
-      </c>
-    </row>
-    <row r="336" spans="1:2">
-      <c r="A336">
-        <v>409.2</v>
-      </c>
-      <c r="B336">
-        <v>6751.88</v>
-      </c>
-    </row>
-    <row r="337" spans="1:2">
-      <c r="A337">
-        <v>409.25</v>
-      </c>
-      <c r="B337">
-        <v>6771.19</v>
-      </c>
-    </row>
-    <row r="338" spans="1:2">
-      <c r="A338">
-        <v>409.3</v>
-      </c>
-      <c r="B338">
-        <v>6786.14</v>
-      </c>
-    </row>
-    <row r="339" spans="1:2">
-      <c r="A339">
-        <v>409.35</v>
-      </c>
-      <c r="B339">
-        <v>6803.19</v>
-      </c>
-    </row>
-    <row r="340" spans="1:2">
-      <c r="A340">
-        <v>409.4</v>
-      </c>
-      <c r="B340">
-        <v>6833.16</v>
-      </c>
-    </row>
-    <row r="341" spans="1:2">
-      <c r="A341">
-        <v>409.45</v>
-      </c>
-      <c r="B341">
-        <v>6871.11</v>
-      </c>
-    </row>
-    <row r="342" spans="1:2">
-      <c r="A342">
-        <v>409.5</v>
-      </c>
-      <c r="B342">
-        <v>6893.57</v>
-      </c>
-    </row>
-    <row r="343" spans="1:2">
-      <c r="A343">
-        <v>409.55</v>
-      </c>
-      <c r="B343">
-        <v>6923.56</v>
-      </c>
-    </row>
-    <row r="344" spans="1:2">
-      <c r="A344">
-        <v>409.6</v>
-      </c>
-      <c r="B344">
-        <v>6946.84</v>
-      </c>
-    </row>
-    <row r="345" spans="1:2">
-      <c r="A345">
-        <v>409.65</v>
-      </c>
-      <c r="B345">
-        <v>6962.82</v>
-      </c>
-    </row>
-    <row r="346" spans="1:2">
-      <c r="A346">
-        <v>409.7</v>
-      </c>
-      <c r="B346">
-        <v>6984.13</v>
-      </c>
-    </row>
-    <row r="347" spans="1:2">
-      <c r="A347">
-        <v>409.75</v>
-      </c>
-      <c r="B347">
-        <v>7018.04</v>
-      </c>
-    </row>
-    <row r="348" spans="1:2">
-      <c r="A348">
-        <v>409.8</v>
-      </c>
-      <c r="B348">
-        <v>7045.64</v>
-      </c>
-    </row>
-    <row r="349" spans="1:2">
-      <c r="A349">
-        <v>409.85</v>
-      </c>
-      <c r="B349">
-        <v>7066.56</v>
-      </c>
-    </row>
-    <row r="350" spans="1:2">
-      <c r="A350">
-        <v>409.9</v>
-      </c>
-      <c r="B350">
-        <v>7091.03</v>
-      </c>
-    </row>
-    <row r="351" spans="1:2">
-      <c r="A351">
-        <v>409.95</v>
-      </c>
-      <c r="B351">
-        <v>7118.27</v>
-      </c>
-    </row>
-    <row r="352" spans="1:2">
-      <c r="A352">
-        <v>410</v>
-      </c>
-      <c r="B352">
-        <v>7146.25</v>
-      </c>
-    </row>
-    <row r="353" spans="1:2">
-      <c r="A353">
-        <v>410.05</v>
-      </c>
-      <c r="B353">
-        <v>7182.21</v>
-      </c>
-    </row>
-    <row r="354" spans="1:2">
-      <c r="A354">
-        <v>410.1</v>
-      </c>
-      <c r="B354">
-        <v>7216.57</v>
-      </c>
-    </row>
-    <row r="355" spans="1:2">
-      <c r="A355">
-        <v>410.15</v>
-      </c>
-      <c r="B355">
-        <v>7263.89</v>
-      </c>
-    </row>
-    <row r="356" spans="1:2">
-      <c r="A356">
-        <v>410.2</v>
-      </c>
-      <c r="B356">
-        <v>7319.74</v>
-      </c>
-    </row>
-    <row r="357" spans="1:2">
-      <c r="A357">
-        <v>410.25</v>
-      </c>
-      <c r="B357">
-        <v>7344.52</v>
-      </c>
-    </row>
-    <row r="358" spans="1:2">
-      <c r="A358">
-        <v>410.3</v>
-      </c>
-      <c r="B358">
-        <v>7372.56</v>
-      </c>
-    </row>
-    <row r="359" spans="1:2">
-      <c r="A359">
-        <v>410.35</v>
-      </c>
-      <c r="B359">
-        <v>7398.36</v>
-      </c>
-    </row>
-    <row r="360" spans="1:2">
-      <c r="A360">
-        <v>410.4</v>
-      </c>
-      <c r="B360">
-        <v>7432.64</v>
-      </c>
-    </row>
-    <row r="361" spans="1:2">
-      <c r="A361">
-        <v>410.45</v>
-      </c>
-      <c r="B361">
-        <v>7480.3</v>
-      </c>
-    </row>
-    <row r="362" spans="1:2">
-      <c r="A362">
-        <v>410.5</v>
-      </c>
-      <c r="B362">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <sortState ref="A2:B362">
-    <sortCondition ref="A2"/>
-  </sortState>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
-</worksheet>
 </file>
</xml_diff>